<commit_message>
ADD: Functionele Analyse en nieuwe scrums
Added Functionele Analyse to Milestone 3.

Added new scums 18/01, 19/01 en new Retrospective
</commit_message>
<xml_diff>
--- a/Documents/Sprint Backlog/Burndown charts.xlsx
+++ b/Documents/Sprint Backlog/Burndown charts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthowest-my.sharepoint.com/personal/jakob_soens_student_howest_be/Documents/Bureaublad/Team Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthowest-my.sharepoint.com/personal/jakob_soens_student_howest_be/Documents/Bureaublad/Team Project/Team-Project-Twister-2.0/Documents/Sprint Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{876129AB-EE64-4BBC-88FB-D4A111D5ACDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{229D60EE-9249-4CE7-A148-BE8D352A5909}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="8_{876129AB-EE64-4BBC-88FB-D4A111D5ACDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AA74EDBF-02D7-459F-9863-D183952C10F9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE3B7036-9469-48C7-8DF3-95661FAFE4C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Ideal</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -908,8 +911,352 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
+              <a:t>Burndown chart</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> III</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$37:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>44206</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44207</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44208</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44209</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44210</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44211</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$37:$B$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CFB9-4924-9527-DA501DC8C704}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="935907696"/>
+        <c:axId val="935903536"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="935907696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="935903536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="935903536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="935907696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>Burndown Chart</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -987,6 +1334,111 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.4934374355769082E-3"/>
+                  <c:y val="-1.8165794238562037E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-37AB-41EF-B336-776A24F20B2B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0389499896923048E-2"/>
+                  <c:y val="-1.5570680775910365E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-37AB-41EF-B336-776A24F20B2B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.4934374355769204E-3"/>
+                  <c:y val="-1.2975567313258598E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-37AB-41EF-B336-776A24F20B2B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.4934374355769204E-3"/>
+                  <c:y val="-1.8165794238562037E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-37AB-41EF-B336-776A24F20B2B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.174664672755295E-3"/>
+                  <c:y val="-2.5951134626517196E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-37AB-41EF-B336-776A24F20B2B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1045,10 +1497,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$N$4:$N$22</c:f>
+              <c:f>Sheet1!$N$4:$N$27</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>44200</c:v>
                 </c:pt>
@@ -1105,30 +1557,72 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44219</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44220</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44221</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44222</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$4:$O$22</c:f>
+              <c:f>Sheet1!$O$4:$O$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>126</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>118</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>107</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1136,7 +1630,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E1FD-4A1E-B0A0-96E50E193356}"/>
+              <c16:uniqueId val="{00000000-37AB-41EF-B336-776A24F20B2B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1180,10 +1674,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$N$4:$N$22</c:f>
+              <c:f>Sheet1!$N$4:$N$27</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>44200</c:v>
                 </c:pt>
@@ -1240,71 +1734,101 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44219</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44220</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44221</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>44222</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$4:$P$22</c:f>
+              <c:f>Sheet1!$P$4:$P$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>126</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>119</c:v>
+                  <c:v>129.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>112</c:v>
+                  <c:v>118.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105</c:v>
+                  <c:v>107.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>98</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>84</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>63</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>56</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>28</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>21</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1313,7 +1837,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E1FD-4A1E-B0A0-96E50E193356}"/>
+              <c16:uniqueId val="{00000001-37AB-41EF-B336-776A24F20B2B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1327,11 +1851,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1910437199"/>
-        <c:axId val="1910436783"/>
+        <c:axId val="2017212336"/>
+        <c:axId val="2017225232"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1910437199"/>
+        <c:axId val="2017212336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1355,11 +1879,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1374,14 +1898,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1910436783"/>
+        <c:crossAx val="2017225232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1910436783"/>
+        <c:axId val="2017225232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1432,7 +1956,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1910437199"/>
+        <c:crossAx val="2017212336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1639,6 +2163,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2646,6 +3210,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3224,23 +4291,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>179614</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>308161</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>113179</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>598714</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>39220</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>189379</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AC62A40-0F01-4250-9634-EEB0CC03DE61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BF69A41-D904-4F1E-BEC8-30389129448F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3253,6 +4320,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>33616</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1119</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>6111</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>132432</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{106BA7C9-ECD1-4C07-A94E-0783AA5ACC68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3558,15 +4661,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC5301-1941-4D4D-9060-7996ECF62373}">
-  <dimension ref="A3:Q25"/>
+  <dimension ref="A2:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <f>43+45+52</f>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N3" t="s">
         <v>2</v>
       </c>
@@ -3577,24 +4686,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
+      <c r="L4">
+        <f>126/17</f>
+        <v>7.4117647058823533</v>
+      </c>
       <c r="N4" s="1">
         <v>44200</v>
       </c>
       <c r="O4">
-        <f>147-21</f>
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="P4">
-        <v>126</v>
-      </c>
-      <c r="Q4">
-        <f>126/18</f>
-        <v>7</v>
+        <v>140</v>
+      </c>
+      <c r="S4">
+        <f>43/4</f>
+        <v>10.75</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44509</v>
       </c>
@@ -3605,15 +4717,19 @@
         <v>44201</v>
       </c>
       <c r="O5">
-        <f>O4-8</f>
-        <v>118</v>
+        <f>O4-C22</f>
+        <v>132</v>
       </c>
       <c r="P5">
-        <f>P4-$Q$4</f>
-        <v>119</v>
+        <f>P4-$S$4</f>
+        <v>129.25</v>
+      </c>
+      <c r="S5">
+        <f>45/5</f>
+        <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44510</v>
       </c>
@@ -3624,15 +4740,19 @@
         <v>44202</v>
       </c>
       <c r="O6">
-        <f>O5-5</f>
-        <v>113</v>
+        <f t="shared" ref="O6:O8" si="0">O5-C23</f>
+        <v>127</v>
       </c>
       <c r="P6">
-        <f t="shared" ref="P6:P22" si="0">P5-$Q$4</f>
-        <v>112</v>
+        <f t="shared" ref="P6:P8" si="1">P5-$S$4</f>
+        <v>118.5</v>
+      </c>
+      <c r="S6">
+        <f>52/8</f>
+        <v>6.5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44511</v>
       </c>
@@ -3643,15 +4763,15 @@
         <v>44203</v>
       </c>
       <c r="O7">
-        <f>O6-6</f>
-        <v>107</v>
+        <f t="shared" si="0"/>
+        <v>121</v>
       </c>
       <c r="P7">
-        <f t="shared" si="0"/>
-        <v>105</v>
+        <f t="shared" si="1"/>
+        <v>107.75</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44512</v>
       </c>
@@ -3662,15 +4782,15 @@
         <v>44204</v>
       </c>
       <c r="O8">
-        <f>O7-19</f>
-        <v>88</v>
+        <f t="shared" si="0"/>
+        <v>102</v>
       </c>
       <c r="P8">
-        <f t="shared" si="0"/>
-        <v>98</v>
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44513</v>
       </c>
@@ -3680,84 +4800,113 @@
       <c r="N9" s="1">
         <v>44205</v>
       </c>
+      <c r="O9">
+        <v>92</v>
+      </c>
       <c r="P9">
-        <f t="shared" si="0"/>
-        <v>91</v>
+        <f>P8</f>
+        <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="N10" s="1">
         <v>44206</v>
       </c>
+      <c r="O10">
+        <v>88</v>
+      </c>
       <c r="P10">
-        <f t="shared" si="0"/>
-        <v>84</v>
+        <f>P9</f>
+        <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="N11" s="1">
         <v>44207</v>
       </c>
+      <c r="O11">
+        <f>O10-C39</f>
+        <v>81</v>
+      </c>
       <c r="P11">
-        <f t="shared" si="0"/>
-        <v>77</v>
+        <f>P10-$S$5</f>
+        <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="N12" s="1">
         <v>44208</v>
       </c>
+      <c r="O12">
+        <f t="shared" ref="O12:O14" si="2">O11-C40</f>
+        <v>70</v>
+      </c>
       <c r="P12">
-        <f t="shared" si="0"/>
-        <v>70</v>
+        <f t="shared" ref="P12:P15" si="3">P11-$S$5</f>
+        <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N13" s="1">
         <v>44209</v>
       </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
       <c r="P13">
-        <f t="shared" si="0"/>
-        <v>63</v>
+        <f t="shared" si="3"/>
+        <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N14" s="1">
         <v>44210</v>
       </c>
+      <c r="O14">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
       <c r="P14">
-        <f t="shared" si="0"/>
-        <v>56</v>
+        <f t="shared" si="3"/>
+        <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N15" s="1">
         <v>44211</v>
       </c>
+      <c r="O15">
+        <v>43</v>
+      </c>
       <c r="P15">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <f t="shared" si="3"/>
+        <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N16" s="1">
         <v>44212</v>
       </c>
+      <c r="O16">
+        <v>43</v>
+      </c>
       <c r="P16">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N17" s="1">
         <v>44213</v>
       </c>
+      <c r="O17">
+        <v>43</v>
+      </c>
       <c r="P17">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -3765,8 +4914,8 @@
         <v>44214</v>
       </c>
       <c r="P18">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <f>P17-$S$6</f>
+        <v>45.5</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3774,8 +4923,8 @@
         <v>44215</v>
       </c>
       <c r="P19">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <f t="shared" ref="P19:P22" si="4">P18-$S$6</f>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -3783,8 +4932,8 @@
         <v>44216</v>
       </c>
       <c r="P20">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f t="shared" si="4"/>
+        <v>32.5</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -3798,8 +4947,8 @@
         <v>44217</v>
       </c>
       <c r="P21">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3809,12 +4958,16 @@
       <c r="B22">
         <v>35</v>
       </c>
+      <c r="C22">
+        <f>B21-B22</f>
+        <v>8</v>
+      </c>
       <c r="N22" s="1">
         <v>44218</v>
       </c>
       <c r="P22">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>19.5</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -3824,6 +4977,17 @@
       <c r="B23">
         <v>30</v>
       </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C25" si="5">B22-B23</f>
+        <v>5</v>
+      </c>
+      <c r="N23" s="1">
+        <v>44219</v>
+      </c>
+      <c r="P23">
+        <f>P22</f>
+        <v>19.5</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -3832,6 +4996,17 @@
       <c r="B24">
         <v>24</v>
       </c>
+      <c r="C24">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="N24" s="1">
+        <v>44220</v>
+      </c>
+      <c r="P24">
+        <f>P22</f>
+        <v>19.5</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -3839,6 +5014,108 @@
       </c>
       <c r="B25">
         <v>5</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="N25" s="1">
+        <v>44221</v>
+      </c>
+      <c r="P25">
+        <f>P24-S$6</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N26" s="1">
+        <v>44222</v>
+      </c>
+      <c r="P26">
+        <f>P25-S$6</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N27" s="1">
+        <v>44223</v>
+      </c>
+      <c r="P27">
+        <f>P26-S$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>44206</v>
+      </c>
+      <c r="B37">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>44207</v>
+      </c>
+      <c r="B38">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <f>B37-B38</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>44208</v>
+      </c>
+      <c r="B39">
+        <v>28</v>
+      </c>
+      <c r="C39">
+        <f>B38-B39</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>44209</v>
+      </c>
+      <c r="B40">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ref="C40:C42" si="6">B39-B40</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>44210</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>44211</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD: New Documentation & new Scrum
Added new documentation Github file & new scrum meeting
</commit_message>
<xml_diff>
--- a/Documents/Sprint Backlog/Burndown charts.xlsx
+++ b/Documents/Sprint Backlog/Burndown charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthowest-my.sharepoint.com/personal/jakob_soens_student_howest_be/Documents/Bureaublad/Team Project/Team-Project-Twister-2.0/Documents/Sprint Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="8_{876129AB-EE64-4BBC-88FB-D4A111D5ACDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AA74EDBF-02D7-459F-9863-D183952C10F9}"/>
+  <xr:revisionPtr revIDLastSave="261" documentId="8_{876129AB-EE64-4BBC-88FB-D4A111D5ACDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{F1F6D4EE-DB10-41F5-AF67-9167A6E5A6E9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE3B7036-9469-48C7-8DF3-95661FAFE4C4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE3B7036-9469-48C7-8DF3-95661FAFE4C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Ideal</t>
   </si>
@@ -46,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -86,7 +88,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -104,7 +106,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -171,7 +173,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -235,7 +237,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-BE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -374,7 +376,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="924596656"/>
@@ -432,7 +434,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="924595408"/>
@@ -480,7 +482,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -494,7 +496,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -556,7 +558,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -620,7 +622,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-BE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -759,7 +761,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="924600400"/>
@@ -817,7 +819,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="924587504"/>
@@ -865,7 +867,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -879,7 +881,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -946,7 +948,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1098,7 +1100,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="935903536"/>
@@ -1156,7 +1158,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="935907696"/>
@@ -1204,7 +1206,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1218,7 +1220,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1285,7 +1287,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1465,7 +1467,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-BE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1895,7 +1897,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2017225232"/>
@@ -1953,7 +1955,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-BE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2017212336"/>
@@ -1995,7 +1997,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-BE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2032,7 +2034,356 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="nl-NL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-BE"/>
+              <a:t>Burndown Chart IV</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$51:$A$60</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>44214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44215</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44216</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44217</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44218</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44220</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44221</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44222</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44223</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$51:$B$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DCE2-4D4F-B131-824BBD1F006F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="678238016"/>
+        <c:axId val="678235392"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="678238016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="678235392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="678235392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-BE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="678238016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-BE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2203,6 +2554,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -3713,6 +4104,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4361,11 +5255,47 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>386603</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>34737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>117662</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>110937</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafiek 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{215B292A-EF18-4EC2-BCFA-F234F54FBD86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4661,10 +5591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC5301-1941-4D4D-9060-7996ECF62373}">
-  <dimension ref="A2:S42"/>
+  <dimension ref="A2:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M51" sqref="M51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5118,6 +6048,87 @@
         <v>3</v>
       </c>
     </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>44214</v>
+      </c>
+      <c r="B51">
+        <v>53</v>
+      </c>
+      <c r="M51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>44215</v>
+      </c>
+      <c r="B52">
+        <f>53-8</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>44216</v>
+      </c>
+      <c r="B53">
+        <f>45-8</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>44217</v>
+      </c>
+      <c r="B54">
+        <f>32</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>44218</v>
+      </c>
+      <c r="B55">
+        <f>22</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>44219</v>
+      </c>
+      <c r="B56">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>44220</v>
+      </c>
+      <c r="B57">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>44221</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>44222</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>44223</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
ADD: Handleidingen, FIX: Documents
Added User manual & Installation manual
Fixed most documents on layout and spelling errors
</commit_message>
<xml_diff>
--- a/Documents/Sprint Backlog/Burndown charts.xlsx
+++ b/Documents/Sprint Backlog/Burndown charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthowest-my.sharepoint.com/personal/jakob_soens_student_howest_be/Documents/Bureaublad/Team Project/Team-Project-Twister-2.0/Documents/Sprint Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{876129AB-EE64-4BBC-88FB-D4A111D5ACDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{F1F6D4EE-DB10-41F5-AF67-9167A6E5A6E9}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="8_{876129AB-EE64-4BBC-88FB-D4A111D5ACDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{745252C4-D184-4BA5-916C-DD2EC728924D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE3B7036-9469-48C7-8DF3-95661FAFE4C4}"/>
+    <workbookView xWindow="4185" yWindow="2190" windowWidth="21600" windowHeight="11385" xr2:uid="{FE3B7036-9469-48C7-8DF3-95661FAFE4C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Ideal</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>a</t>
   </si>
 </sst>
 </file>
@@ -88,7 +85,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -106,7 +103,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -173,7 +170,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -237,7 +234,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-BE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -376,7 +373,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="924596656"/>
@@ -434,7 +431,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="924595408"/>
@@ -482,7 +479,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -496,7 +493,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -558,7 +555,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -622,7 +619,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-BE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -761,7 +758,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="924600400"/>
@@ -819,7 +816,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="924587504"/>
@@ -867,7 +864,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -881,7 +878,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -948,7 +945,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -985,6 +982,126 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3888888888888914E-2"/>
+                  <c:y val="-4.1666666666666706E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-BD54-49FF-A34B-BCB77AB8E808}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1111111111111112E-2"/>
+                  <c:y val="-3.2407407407407406E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-BD54-49FF-A34B-BCB77AB8E808}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.2222222222222223E-2"/>
+                  <c:y val="-5.0925925925926097E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-BD54-49FF-A34B-BCB77AB8E808}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$37:$A$42</c:f>
@@ -1100,7 +1217,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="935903536"/>
@@ -1158,7 +1275,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="935907696"/>
@@ -1206,7 +1323,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1220,7 +1337,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1287,7 +1404,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1312,7 +1429,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1337,11 +1454,32 @@
           </c:marker>
           <c:dLbls>
             <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.0996206819536195E-3"/>
+                  <c:y val="-2.6153126348842343E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.4934374355769082E-3"/>
-                  <c:y val="-1.8165794238562037E-2"/>
+                  <c:x val="-1.429940392878426E-2"/>
+                  <c:y val="-2.6153126348842318E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1361,8 +1499,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.0389499896923048E-2"/>
-                  <c:y val="-1.5570680775910365E-2"/>
+                  <c:x val="-1.0399566493661279E-2"/>
+                  <c:y val="-2.3537813713958158E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1382,8 +1520,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.4934374355769204E-3"/>
-                  <c:y val="-1.2975567313258598E-2"/>
+                  <c:x val="-1.0399566493661304E-2"/>
+                  <c:y val="-1.8307188444189642E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1403,8 +1541,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.4934374355769204E-3"/>
-                  <c:y val="-1.8165794238562037E-2"/>
+                  <c:x val="-9.0996206819536438E-3"/>
+                  <c:y val="-2.3537813713958109E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1424,8 +1562,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.174664672755295E-3"/>
-                  <c:y val="-2.5951134626517196E-2"/>
+                  <c:x val="-1.8201352798264892E-2"/>
+                  <c:y val="-2.3520574128363423E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1438,6 +1576,336 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-37AB-41EF-B336-776A24F20B2B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.1070277570732619E-3"/>
+                  <c:y val="-2.6325133641510182E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.8060237917771287E-3"/>
+                  <c:y val="-2.3692620277359071E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.107020234897777E-3"/>
+                  <c:y val="-1.7999325078575573E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.8060237917771287E-3"/>
+                  <c:y val="-1.8427593549057191E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1710176758372149E-2"/>
+                  <c:y val="-1.8111429559952291E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1709035687665622E-2"/>
+                  <c:y val="-2.3692620277359119E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4974191405871516E-2"/>
+                  <c:y val="-2.5960464158443698E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="2.0990033107459751E-2"/>
+                      <c:h val="4.118389549624555E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.2383392547317495E-2"/>
+                  <c:y val="1.5851639224833569E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.2135890994219344E-2"/>
+                  <c:y val="2.0611220050335291E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.2198014722249783E-2"/>
+                  <c:y val="2.3356021163865572E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.3685427546888498E-2"/>
+                  <c:y val="1.7438147089929919E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8907119371920706E-2"/>
+                  <c:y val="1.9024654955026272E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8229557289357202E-2"/>
+                  <c:y val="2.0611220050335197E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-7C3A-44BF-B5B0-035C58B456D5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.5625334819448854E-2"/>
+                  <c:y val="-3.0916830075502794E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-7C3A-44BF-B5B0-035C58B456D5}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1467,7 +1935,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="nl-BE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1580,7 +2048,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$4:$O$27</c:f>
+              <c:f>Sheet1!$Q$4:$Q$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1600,31 +2068,61 @@
                   <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>92</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>81</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>70</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43</c:v>
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1651,7 +2149,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="12700" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1660,7 +2158,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="plus"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -1897,7 +2395,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2017225232"/>
@@ -1955,7 +2453,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2017212336"/>
@@ -1997,7 +2495,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2034,7 +2532,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2048,7 +2546,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2110,7 +2608,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-BE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2193,10 +2691,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>53</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>37</c:v>
@@ -2208,10 +2706,10 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2277,7 +2775,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="678235392"/>
@@ -2335,7 +2833,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-BE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="678238016"/>
@@ -2383,7 +2881,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-BE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5222,15 +5720,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>33616</xdr:colOff>
+      <xdr:colOff>33615</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>1119</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>6111</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>132432</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>510267</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>162127</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5295,7 +5793,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5593,8 +6091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC5301-1941-4D4D-9060-7996ECF62373}">
   <dimension ref="A2:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="92" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="O44" sqref="O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5615,6 +6113,9 @@
       <c r="P3" t="s">
         <v>0</v>
       </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -5631,6 +6132,9 @@
       <c r="P4">
         <v>140</v>
       </c>
+      <c r="Q4">
+        <v>140</v>
+      </c>
       <c r="S4">
         <f>43/4</f>
         <v>10.75</v>
@@ -5654,6 +6158,10 @@
         <f>P4-$S$4</f>
         <v>129.25</v>
       </c>
+      <c r="Q5">
+        <f>Q4-C22</f>
+        <v>132</v>
+      </c>
       <c r="S5">
         <f>45/5</f>
         <v>9</v>
@@ -5666,6 +6174,10 @@
       <c r="B6">
         <v>18</v>
       </c>
+      <c r="C6">
+        <f>B5-B6</f>
+        <v>3</v>
+      </c>
       <c r="N6" s="1">
         <v>44202</v>
       </c>
@@ -5676,6 +6188,10 @@
       <c r="P6">
         <f t="shared" ref="P6:P8" si="1">P5-$S$4</f>
         <v>118.5</v>
+      </c>
+      <c r="Q6">
+        <f>Q5-C23</f>
+        <v>127</v>
       </c>
       <c r="S6">
         <f>52/8</f>
@@ -5689,6 +6205,10 @@
       <c r="B7">
         <v>15</v>
       </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C9" si="2">B6-B7</f>
+        <v>3</v>
+      </c>
       <c r="N7" s="1">
         <v>44203</v>
       </c>
@@ -5699,6 +6219,10 @@
       <c r="P7">
         <f t="shared" si="1"/>
         <v>107.75</v>
+      </c>
+      <c r="Q7">
+        <f>Q6-C24</f>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -5708,6 +6232,10 @@
       <c r="B8">
         <v>8</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
       <c r="N8" s="1">
         <v>44204</v>
       </c>
@@ -5718,6 +6246,10 @@
       <c r="P8">
         <f t="shared" si="1"/>
         <v>97</v>
+      </c>
+      <c r="Q8">
+        <f>Q7-C25</f>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -5727,6 +6259,10 @@
       <c r="B9">
         <v>0</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
       <c r="N9" s="1">
         <v>44205</v>
       </c>
@@ -5736,6 +6272,9 @@
       <c r="P9">
         <f>P8</f>
         <v>97</v>
+      </c>
+      <c r="Q9">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -5750,6 +6289,9 @@
         <f>P9</f>
         <v>97</v>
       </c>
+      <c r="Q10">
+        <v>102</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -5764,6 +6306,10 @@
         <f>P10-$S$5</f>
         <v>88</v>
       </c>
+      <c r="Q11">
+        <f t="shared" ref="Q11:Q17" si="3">Q10-C38</f>
+        <v>92</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -5771,12 +6317,16 @@
         <v>44208</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12:O14" si="2">O11-C40</f>
+        <f t="shared" ref="O12:O14" si="4">O11-C40</f>
         <v>70</v>
       </c>
       <c r="P12">
-        <f t="shared" ref="P12:P15" si="3">P11-$S$5</f>
+        <f t="shared" ref="P12:P15" si="5">P11-$S$5</f>
         <v>79</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="3"/>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -5784,12 +6334,16 @@
         <v>44209</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>56</v>
       </c>
       <c r="P13">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="Q13">
         <f t="shared" si="3"/>
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -5797,12 +6351,16 @@
         <v>44210</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
       <c r="P14">
+        <f t="shared" si="5"/>
+        <v>61</v>
+      </c>
+      <c r="Q14">
         <f t="shared" si="3"/>
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -5813,8 +6371,12 @@
         <v>43</v>
       </c>
       <c r="P15">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="Q15">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -5827,8 +6389,12 @@
       <c r="P16">
         <v>52</v>
       </c>
+      <c r="Q16">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N17" s="1">
         <v>44213</v>
       </c>
@@ -5838,8 +6404,12 @@
       <c r="P17">
         <v>52</v>
       </c>
+      <c r="Q17">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N18" s="1">
         <v>44214</v>
       </c>
@@ -5847,26 +6417,38 @@
         <f>P17-$S$6</f>
         <v>45.5</v>
       </c>
+      <c r="Q18">
+        <f t="shared" ref="Q18:Q27" si="6">Q17-C52</f>
+        <v>39</v>
+      </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N19" s="1">
         <v>44215</v>
       </c>
       <c r="P19">
-        <f t="shared" ref="P19:P22" si="4">P18-$S$6</f>
+        <f t="shared" ref="P19:P22" si="7">P18-$S$6</f>
         <v>39</v>
       </c>
+      <c r="Q19">
+        <f t="shared" si="6"/>
+        <v>37</v>
+      </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N20" s="1">
         <v>44216</v>
       </c>
       <c r="P20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>32.5</v>
       </c>
+      <c r="Q20">
+        <f t="shared" si="6"/>
+        <v>32</v>
+      </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44200</v>
       </c>
@@ -5877,11 +6459,15 @@
         <v>44217</v>
       </c>
       <c r="P21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
+      <c r="Q21">
+        <f t="shared" si="6"/>
+        <v>22</v>
+      </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44201</v>
       </c>
@@ -5896,11 +6482,15 @@
         <v>44218</v>
       </c>
       <c r="P22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>19.5</v>
       </c>
+      <c r="Q22">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44202</v>
       </c>
@@ -5908,7 +6498,7 @@
         <v>30</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:C25" si="5">B22-B23</f>
+        <f t="shared" ref="C23:C25" si="8">B22-B23</f>
         <v>5</v>
       </c>
       <c r="N23" s="1">
@@ -5918,8 +6508,12 @@
         <f>P22</f>
         <v>19.5</v>
       </c>
+      <c r="Q23">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44203</v>
       </c>
@@ -5927,7 +6521,7 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="N24" s="1">
@@ -5937,8 +6531,12 @@
         <f>P22</f>
         <v>19.5</v>
       </c>
+      <c r="Q24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44204</v>
       </c>
@@ -5946,7 +6544,7 @@
         <v>5</v>
       </c>
       <c r="C25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="N25" s="1">
@@ -5956,8 +6554,12 @@
         <f>P24-S$6</f>
         <v>13</v>
       </c>
+      <c r="Q25">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N26" s="1">
         <v>44222</v>
       </c>
@@ -5965,8 +6567,12 @@
         <f>P25-S$6</f>
         <v>6.5</v>
       </c>
+      <c r="Q26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="N27" s="1">
         <v>44223</v>
       </c>
@@ -5974,8 +6580,12 @@
         <f>P26-S$6</f>
         <v>0</v>
       </c>
+      <c r="Q27">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P31" t="s">
         <v>3</v>
       </c>
@@ -6020,7 +6630,7 @@
         <v>17</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:C42" si="6">B39-B40</f>
+        <f t="shared" ref="C40:C44" si="9">B39-B40</f>
         <v>11</v>
       </c>
     </row>
@@ -6032,7 +6642,7 @@
         <v>3</v>
       </c>
       <c r="C41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
     </row>
@@ -6044,34 +6654,56 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>44212</v>
+      </c>
+      <c r="B43">
+        <v>-5</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>-10</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44214</v>
       </c>
       <c r="B51">
-        <v>53</v>
-      </c>
-      <c r="M51" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44215</v>
       </c>
       <c r="B52">
-        <f>53-8</f>
-        <v>45</v>
+        <f>B51-8</f>
+        <v>39</v>
+      </c>
+      <c r="C52">
+        <f>B51-B52</f>
+        <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44216</v>
       </c>
@@ -6079,8 +6711,12 @@
         <f>45-8</f>
         <v>37</v>
       </c>
+      <c r="C53">
+        <f t="shared" ref="C53:C60" si="10">B52-B53</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44217</v>
       </c>
@@ -6088,8 +6724,12 @@
         <f>32</f>
         <v>32</v>
       </c>
+      <c r="C54">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44218</v>
       </c>
@@ -6097,36 +6737,60 @@
         <f>22</f>
         <v>22</v>
       </c>
+      <c r="C55">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44219</v>
       </c>
       <c r="B56">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="10"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44220</v>
       </c>
       <c r="B57">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44221</v>
       </c>
+      <c r="C58">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44222</v>
       </c>
+      <c r="C59">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44223</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD: new Scrum, FIX: Handleidingen
Added new Scrum meeting 25/01
Fixed handleidingen
</commit_message>
<xml_diff>
--- a/Documents/Sprint Backlog/Burndown charts.xlsx
+++ b/Documents/Sprint Backlog/Burndown charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthowest-my.sharepoint.com/personal/jakob_soens_student_howest_be/Documents/Bureaublad/Team Project/Team-Project-Twister-2.0/Documents/Sprint Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="8_{876129AB-EE64-4BBC-88FB-D4A111D5ACDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{745252C4-D184-4BA5-916C-DD2EC728924D}"/>
+  <xr:revisionPtr revIDLastSave="343" documentId="8_{876129AB-EE64-4BBC-88FB-D4A111D5ACDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6CAD0148-303A-4B1C-B139-09C1EF02063C}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="2190" windowWidth="21600" windowHeight="11385" xr2:uid="{FE3B7036-9469-48C7-8DF3-95661FAFE4C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE3B7036-9469-48C7-8DF3-95661FAFE4C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2092,31 +2092,31 @@
                   <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>47</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -2710,6 +2710,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6091,8 +6094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FC5301-1941-4D4D-9060-7996ECF62373}">
   <dimension ref="A2:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="92" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="O44" sqref="O44"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19:Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6405,8 +6408,7 @@
         <v>52</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="3"/>
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -6418,8 +6420,8 @@
         <v>45.5</v>
       </c>
       <c r="Q18">
-        <f t="shared" ref="Q18:Q27" si="6">Q17-C52</f>
-        <v>39</v>
+        <f>Q17-C44</f>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -6427,12 +6429,12 @@
         <v>44215</v>
       </c>
       <c r="P19">
-        <f t="shared" ref="P19:P22" si="7">P18-$S$6</f>
+        <f t="shared" ref="P19:P22" si="6">P18-$S$6</f>
         <v>39</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="6"/>
-        <v>37</v>
+        <f>Q18-C52</f>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -6440,12 +6442,12 @@
         <v>44216</v>
       </c>
       <c r="P20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>32.5</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="6"/>
-        <v>32</v>
+        <f t="shared" ref="Q20:Q27" si="7">Q19-C53</f>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -6459,12 +6461,12 @@
         <v>44217</v>
       </c>
       <c r="P21">
+        <f t="shared" si="6"/>
+        <v>26</v>
+      </c>
+      <c r="Q21">
         <f t="shared" si="7"/>
-        <v>26</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="6"/>
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -6482,12 +6484,12 @@
         <v>44218</v>
       </c>
       <c r="P22">
+        <f t="shared" si="6"/>
+        <v>19.5</v>
+      </c>
+      <c r="Q22">
         <f t="shared" si="7"/>
-        <v>19.5</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -6509,8 +6511,8 @@
         <v>19.5</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="6"/>
-        <v>16</v>
+        <f t="shared" si="7"/>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -6532,8 +6534,8 @@
         <v>19.5</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -6555,8 +6557,8 @@
         <v>13</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -6568,7 +6570,7 @@
         <v>6.5</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6581,7 +6583,7 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -6770,9 +6772,12 @@
       <c r="A58" s="1">
         <v>44221</v>
       </c>
+      <c r="B58">
+        <v>10</v>
+      </c>
       <c r="C58">
         <f t="shared" si="10"/>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -6781,7 +6786,7 @@
       </c>
       <c r="C59">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>